<commit_message>
corret the pd.cut issue
</commit_message>
<xml_diff>
--- a/personal-my-work/panda_challenge_analysis.xlsx
+++ b/personal-my-work/panda_challenge_analysis.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>School Type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>size</t>
+          <t>Total Students</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -466,12 +466,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>average_math_score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>average_reading_score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -491,9 +491,9 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Huang High School</t>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Bailey High School</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -502,106 +502,118 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2917</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1910635</v>
-      </c>
-      <c r="E2" t="n">
-        <v>655</v>
+        <v>4976</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$3,124,928.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>$628.00</t>
+        </is>
       </c>
       <c r="F2" t="n">
-        <v>76.62941378128214</v>
+        <v>77.04843247588424</v>
       </c>
       <c r="G2" t="n">
-        <v>81.18272197463148</v>
+        <v>81.03396302250803</v>
       </c>
       <c r="H2" t="n">
-        <v>65.68392183750429</v>
+        <v>66.68006430868168</v>
       </c>
       <c r="I2" t="n">
-        <v>81.31642098045937</v>
+        <v>81.93327974276528</v>
       </c>
       <c r="J2" t="n">
-        <v>53.51388412752829</v>
+        <v>54.64228295819936</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cabrera High School</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1858</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$1,081,356.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$582.00</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>83.06189451022605</v>
+      </c>
+      <c r="G3" t="n">
+        <v>83.97578040904197</v>
+      </c>
+      <c r="H3" t="n">
+        <v>94.1334768568353</v>
+      </c>
+      <c r="I3" t="n">
+        <v>97.03982777179763</v>
+      </c>
+      <c r="J3" t="n">
+        <v>91.33476856835307</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>Figueroa High School</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>District</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>2949</v>
       </c>
-      <c r="D3" t="n">
-        <v>1884411</v>
-      </c>
-      <c r="E3" t="n">
-        <v>639</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$1,884,411.00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$639.00</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
         <v>76.71176670057646</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G4" t="n">
         <v>81.15801966768396</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H4" t="n">
         <v>65.98847066802306</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I4" t="n">
         <v>80.73923363852153</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J4" t="n">
         <v>53.20447609359105</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Shelton High School</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1761</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1056600</v>
-      </c>
-      <c r="E4" t="n">
-        <v>600</v>
-      </c>
-      <c r="F4" t="n">
-        <v>83.35945485519591</v>
-      </c>
-      <c r="G4" t="n">
-        <v>83.72572402044293</v>
-      </c>
-      <c r="H4" t="n">
-        <v>93.86712095400341</v>
-      </c>
-      <c r="I4" t="n">
-        <v>95.85462805224304</v>
-      </c>
-      <c r="J4" t="n">
-        <v>89.89210675752413</v>
-      </c>
-    </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hernandez High School</t>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ford High School</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -610,32 +622,36 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4635</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3022020</v>
-      </c>
-      <c r="E5" t="n">
-        <v>652</v>
+        <v>2739</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$1,763,916.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$644.00</t>
+        </is>
       </c>
       <c r="F5" t="n">
-        <v>77.28975188781014</v>
+        <v>77.10259218692954</v>
       </c>
       <c r="G5" t="n">
-        <v>80.9344120819849</v>
+        <v>80.74625775830594</v>
       </c>
       <c r="H5" t="n">
-        <v>66.7529665587918</v>
+        <v>68.3096020445418</v>
       </c>
       <c r="I5" t="n">
-        <v>80.86299892125135</v>
+        <v>79.29901423877328</v>
       </c>
       <c r="J5" t="n">
-        <v>53.52750809061489</v>
+        <v>54.2898868200073</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Griffin High School</t>
         </is>
@@ -648,11 +664,15 @@
       <c r="C6" t="n">
         <v>1468</v>
       </c>
-      <c r="D6" t="n">
-        <v>917500</v>
-      </c>
-      <c r="E6" t="n">
-        <v>625</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$917,500.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$625.00</t>
+        </is>
       </c>
       <c r="F6" t="n">
         <v>83.35149863760218</v>
@@ -671,81 +691,89 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Wilson High School</t>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Hernandez High School</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>District</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>4635</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$3,022,020.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$652.00</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>77.28975188781014</v>
+      </c>
+      <c r="G7" t="n">
+        <v>80.9344120819849</v>
+      </c>
+      <c r="H7" t="n">
+        <v>66.7529665587918</v>
+      </c>
+      <c r="I7" t="n">
+        <v>80.86299892125135</v>
+      </c>
+      <c r="J7" t="n">
+        <v>53.52750809061489</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Holden High School</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Charter</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>2283</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1319574</v>
-      </c>
-      <c r="E7" t="n">
-        <v>578</v>
-      </c>
-      <c r="F7" t="n">
-        <v>83.2742006132282</v>
-      </c>
-      <c r="G7" t="n">
-        <v>83.98948751642575</v>
-      </c>
-      <c r="H7" t="n">
-        <v>93.86771791502409</v>
-      </c>
-      <c r="I7" t="n">
-        <v>96.53964082347788</v>
-      </c>
-      <c r="J7" t="n">
-        <v>90.5825667980727</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Cabrera High School</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
       <c r="C8" t="n">
-        <v>1858</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1081356</v>
-      </c>
-      <c r="E8" t="n">
-        <v>582</v>
+        <v>427</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$248,087.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$581.00</t>
+        </is>
       </c>
       <c r="F8" t="n">
-        <v>83.06189451022605</v>
+        <v>83.80327868852459</v>
       </c>
       <c r="G8" t="n">
-        <v>83.97578040904197</v>
+        <v>83.81498829039812</v>
       </c>
       <c r="H8" t="n">
-        <v>94.1334768568353</v>
+        <v>92.50585480093677</v>
       </c>
       <c r="I8" t="n">
-        <v>97.03982777179763</v>
+        <v>96.25292740046838</v>
       </c>
       <c r="J8" t="n">
-        <v>91.33476856835307</v>
+        <v>89.22716627634661</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Bailey High School</t>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Huang High School</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -754,68 +782,76 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4976</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3124928</v>
-      </c>
-      <c r="E9" t="n">
-        <v>628</v>
+        <v>2917</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$1,910,635.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$655.00</t>
+        </is>
       </c>
       <c r="F9" t="n">
-        <v>77.04843247588424</v>
+        <v>76.62941378128214</v>
       </c>
       <c r="G9" t="n">
-        <v>81.03396302250803</v>
+        <v>81.18272197463148</v>
       </c>
       <c r="H9" t="n">
-        <v>66.68006430868168</v>
+        <v>65.68392183750429</v>
       </c>
       <c r="I9" t="n">
-        <v>81.93327974276528</v>
+        <v>81.31642098045937</v>
       </c>
       <c r="J9" t="n">
-        <v>54.64228295819936</v>
+        <v>53.51388412752829</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Holden High School</t>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Johnson High School</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Charter</t>
+          <t>District</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>427</v>
-      </c>
-      <c r="D10" t="n">
-        <v>248087</v>
-      </c>
-      <c r="E10" t="n">
-        <v>581</v>
+        <v>4761</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$3,094,650.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>$650.00</t>
+        </is>
       </c>
       <c r="F10" t="n">
-        <v>83.80327868852459</v>
+        <v>77.07246376811594</v>
       </c>
       <c r="G10" t="n">
-        <v>83.81498829039812</v>
+        <v>80.96639361478681</v>
       </c>
       <c r="H10" t="n">
-        <v>92.50585480093677</v>
+        <v>66.05755093467759</v>
       </c>
       <c r="I10" t="n">
-        <v>96.25292740046838</v>
+        <v>81.2224322621298</v>
       </c>
       <c r="J10" t="n">
-        <v>89.22716627634661</v>
+        <v>53.53917244276413</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Pena High School</t>
         </is>
@@ -828,11 +864,15 @@
       <c r="C11" t="n">
         <v>962</v>
       </c>
-      <c r="D11" t="n">
-        <v>585858</v>
-      </c>
-      <c r="E11" t="n">
-        <v>609</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$585,858.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$609.00</t>
+        </is>
       </c>
       <c r="F11" t="n">
         <v>83.83991683991684</v>
@@ -851,183 +891,203 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Rodriguez High School</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3999</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$2,547,363.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>$637.00</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>76.84271067766942</v>
+      </c>
+      <c r="G12" t="n">
+        <v>80.74468617154288</v>
+      </c>
+      <c r="H12" t="n">
+        <v>66.36659164791197</v>
+      </c>
+      <c r="I12" t="n">
+        <v>80.22005501375344</v>
+      </c>
+      <c r="J12" t="n">
+        <v>52.98824706176544</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Shelton High School</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1761</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$1,056,600.00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>$600.00</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>83.35945485519591</v>
+      </c>
+      <c r="G13" t="n">
+        <v>83.72572402044293</v>
+      </c>
+      <c r="H13" t="n">
+        <v>93.86712095400341</v>
+      </c>
+      <c r="I13" t="n">
+        <v>95.85462805224304</v>
+      </c>
+      <c r="J13" t="n">
+        <v>89.89210675752413</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Thomas High School</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>1635</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$1,043,130.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$638.00</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>83.41834862385321</v>
+      </c>
+      <c r="G14" t="n">
+        <v>83.84892966360856</v>
+      </c>
+      <c r="H14" t="n">
+        <v>93.27217125382263</v>
+      </c>
+      <c r="I14" t="n">
+        <v>97.30886850152905</v>
+      </c>
+      <c r="J14" t="n">
+        <v>90.94801223241591</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Wilson High School</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>2283</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$1,319,574.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>$578.00</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>83.2742006132282</v>
+      </c>
+      <c r="G15" t="n">
+        <v>83.98948751642575</v>
+      </c>
+      <c r="H15" t="n">
+        <v>93.86771791502409</v>
+      </c>
+      <c r="I15" t="n">
+        <v>96.53964082347788</v>
+      </c>
+      <c r="J15" t="n">
+        <v>90.5825667980727</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Wright High School</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>Charter</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C16" t="n">
         <v>1800</v>
       </c>
-      <c r="D12" t="n">
-        <v>1049400</v>
-      </c>
-      <c r="E12" t="n">
-        <v>583</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$1,049,400.00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>$583.00</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>83.68222222222222</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G16" t="n">
         <v>83.955</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H16" t="n">
         <v>93.33333333333333</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I16" t="n">
         <v>96.61111111111111</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J16" t="n">
         <v>90.33333333333333</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Rodriguez High School</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>3999</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2547363</v>
-      </c>
-      <c r="E13" t="n">
-        <v>637</v>
-      </c>
-      <c r="F13" t="n">
-        <v>76.84271067766942</v>
-      </c>
-      <c r="G13" t="n">
-        <v>80.74468617154288</v>
-      </c>
-      <c r="H13" t="n">
-        <v>66.36659164791197</v>
-      </c>
-      <c r="I13" t="n">
-        <v>80.22005501375344</v>
-      </c>
-      <c r="J13" t="n">
-        <v>52.98824706176544</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Johnson High School</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>4761</v>
-      </c>
-      <c r="D14" t="n">
-        <v>3094650</v>
-      </c>
-      <c r="E14" t="n">
-        <v>650</v>
-      </c>
-      <c r="F14" t="n">
-        <v>77.07246376811594</v>
-      </c>
-      <c r="G14" t="n">
-        <v>80.96639361478681</v>
-      </c>
-      <c r="H14" t="n">
-        <v>66.05755093467759</v>
-      </c>
-      <c r="I14" t="n">
-        <v>81.2224322621298</v>
-      </c>
-      <c r="J14" t="n">
-        <v>53.53917244276413</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Ford High School</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>2739</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1763916</v>
-      </c>
-      <c r="E15" t="n">
-        <v>644</v>
-      </c>
-      <c r="F15" t="n">
-        <v>77.10259218692954</v>
-      </c>
-      <c r="G15" t="n">
-        <v>80.74625775830594</v>
-      </c>
-      <c r="H15" t="n">
-        <v>68.3096020445418</v>
-      </c>
-      <c r="I15" t="n">
-        <v>79.29901423877328</v>
-      </c>
-      <c r="J15" t="n">
-        <v>54.2898868200073</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Thomas High School</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1635</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1043130</v>
-      </c>
-      <c r="E16" t="n">
-        <v>638</v>
-      </c>
-      <c r="F16" t="n">
-        <v>83.41834862385321</v>
-      </c>
-      <c r="G16" t="n">
-        <v>83.84892966360856</v>
-      </c>
-      <c r="H16" t="n">
-        <v>93.27217125382263</v>
-      </c>
-      <c r="I16" t="n">
-        <v>97.30886850152905</v>
-      </c>
-      <c r="J16" t="n">
-        <v>90.94801223241591</v>
       </c>
     </row>
   </sheetData>
@@ -1041,7 +1101,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,234 +1110,309 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>9th</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>10th</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>11th</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>12th</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Bailey High School</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>77.08367626886145</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>76.99677158999192</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>77.51558752997602</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>76.49221789883268</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cabrera High School</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>83.09469696969697</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>83.15450643776823</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>82.7655601659751</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>83.27748691099477</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Figueroa High School</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>76.40303738317758</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>76.53997378768021</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>76.88434414668548</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>77.15136876006441</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ford High School</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>77.36134453781513</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>77.67231638418079</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>76.91805766312595</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>76.1799628942486</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Griffin High School</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>82.0440097799511</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>84.22906403940887</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>83.84210526315789</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>83.35616438356165</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Hernandez High School</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>77.43849493487699</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>77.33740831295843</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>77.13602941176471</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>77.18656716417911</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Holden High School</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>83.78740157480316</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>83.42982456140351</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>85</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>82.85542168674699</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Huang High School</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>77.02725118483413</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>75.90873533246415</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>76.44660194174757</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>77.22564102564102</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Johnson High School</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>77.18785714285714</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>76.69111654441728</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>77.49165275459099</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>76.86324786324786</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Pena High School</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>83.62545454545455</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>83.372</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>84.328125</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>84.12154696132596</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Rodriguez High School</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>76.85996563573883</v>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>76.6125</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>76.39562624254474</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>77.69074778200253</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Shelton High School</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>83.42075471698114</v>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>82.91741071428571</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>83.38349514563107</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>83.77897574123989</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Thomas High School</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>83.59002169197397</v>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>83.08788598574822</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>83.49879518072289</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>83.49704142011835</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Wilson High School</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>83.08557844690966</v>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>83.72442244224422</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>83.19532554257096</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>83.03579418344519</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Wright High School</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>83.26470588235294</v>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>84.01028806584362</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>83.8367816091954</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>83.6449864498645</v>
       </c>
     </row>
@@ -1292,7 +1427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1301,234 +1436,309 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>9th</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>10th</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>11th</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>12th</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Bailey High School</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>81.30315500685872</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>80.90718321226795</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>80.94564348521183</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>80.91245136186771</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cabrera High School</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>83.67613636363636</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>84.25321888412017</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>83.78838174273859</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>84.28795811518324</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Figueroa High School</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>81.19859813084112</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>81.40891218872871</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>80.64033850493654</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>81.38486312399355</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ford High School</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>80.63265306122449</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>81.26271186440678</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>80.40364188163885</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>80.66233766233766</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Griffin High School</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>83.36919315403424</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>83.70689655172414</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>84.28808864265928</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>84.01369863013699</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Hernandez High School</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>80.86685962373372</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>80.66014669926651</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>81.39613970588235</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>80.85714285714286</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Holden High School</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>83.67716535433071</v>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>83.32456140350877</v>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>83.81553398058253</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>84.6987951807229</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Huang High School</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>81.29028436018957</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>81.51238591916558</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>81.41747572815534</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>80.3059829059829</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Johnson High School</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>81.26071428571429</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>80.77343113284434</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>80.61602671118531</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>81.2275641025641</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Pena High School</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>83.80727272727273</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>83.61199999999999</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>84.3359375</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>84.59116022099448</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Rodriguez High School</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>80.99312714776632</v>
       </c>
-      <c r="B12" t="n">
+      <c r="C12" t="n">
         <v>80.62980769230769</v>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>80.86481113320079</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>80.3764258555133</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Shelton High School</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>84.12264150943396</v>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>83.44196428571429</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>84.37378640776699</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>82.78167115902966</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Thomas High School</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>83.72885032537961</v>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>84.25415676959619</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>83.58554216867469</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>83.83136094674556</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Wilson High School</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
         <v>83.93977812995246</v>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>84.02145214521452</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>83.76460767946578</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>84.31767337807607</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Wright High School</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
         <v>83.83333333333333</v>
       </c>
-      <c r="B16" t="n">
+      <c r="C16" t="n">
         <v>83.81275720164609</v>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>84.15632183908046</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>84.07317073170732</v>
       </c>
     </row>
@@ -1543,7 +1753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1554,96 +1764,121 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Spending Ranges (Per Student)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Average Math Score</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Average Reading Score</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>% Passing Math</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>% Passing Reading</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>% Overall Passing</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>$585-630</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>81.8998257021498</v>
+      </c>
+      <c r="C2" t="n">
+        <v>83.15528577020937</v>
+      </c>
+      <c r="D2" t="n">
+        <v>87.13353760737169</v>
+      </c>
+      <c r="E2" t="n">
+        <v>92.71820457965273</v>
+      </c>
+      <c r="F2" t="n">
+        <v>81.418596324284</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>$630-645</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>78.51885454725715</v>
+      </c>
+      <c r="C3" t="n">
+        <v>81.62447331528534</v>
+      </c>
+      <c r="D3" t="n">
+        <v>73.48420890357487</v>
+      </c>
+      <c r="E3" t="n">
+        <v>84.39179284814432</v>
+      </c>
+      <c r="F3" t="n">
+        <v>62.85765555194492</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>$645-680</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>76.99720981240274</v>
+      </c>
+      <c r="C4" t="n">
+        <v>81.02784255713441</v>
+      </c>
+      <c r="D4" t="n">
+        <v>66.16481311032456</v>
+      </c>
+      <c r="E4" t="n">
+        <v>81.13395072128017</v>
+      </c>
+      <c r="F4" t="n">
+        <v>53.5268548869691</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>&lt;$585</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>83.45539900855027</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C5" t="n">
         <v>83.93381405396646</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D5" t="n">
         <v>93.46009572653237</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E5" t="n">
         <v>96.61087677671375</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F5" t="n">
         <v>90.36945874402643</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>81.8998257021498</v>
-      </c>
-      <c r="B3" t="n">
-        <v>83.15528577020937</v>
-      </c>
-      <c r="C3" t="n">
-        <v>87.13353760737169</v>
-      </c>
-      <c r="D3" t="n">
-        <v>92.71820457965273</v>
-      </c>
-      <c r="E3" t="n">
-        <v>81.418596324284</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>78.51885454725715</v>
-      </c>
-      <c r="B4" t="n">
-        <v>81.62447331528534</v>
-      </c>
-      <c r="C4" t="n">
-        <v>73.48420890357487</v>
-      </c>
-      <c r="D4" t="n">
-        <v>84.39179284814432</v>
-      </c>
-      <c r="E4" t="n">
-        <v>62.85765555194492</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>76.99720981240274</v>
-      </c>
-      <c r="B5" t="n">
-        <v>81.02784255713441</v>
-      </c>
-      <c r="C5" t="n">
-        <v>66.16481311032456</v>
-      </c>
-      <c r="D5" t="n">
-        <v>81.13395072128017</v>
-      </c>
-      <c r="E5" t="n">
-        <v>53.5268548869691</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +1892,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1668,78 +1903,98 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>School Size</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Average Math Score</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Average Reading Score</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>% Passing Math</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>% Passing Reading</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>% Overall Passing</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Large (2000-5000)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>77.746416511437</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>81.34449272598371</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>69.96336073939453</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>82.76663445264148</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>58.28600304906789</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Medium (1000-2000)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>83.37468376981991</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>83.86443831725629</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>93.59969459404036</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>96.7906800028675</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>90.62153518649967</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Small (&lt;1000)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>83.82159776422071</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>83.92984341754834</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>93.55022469776569</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>96.09943667320717</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>89.88385340844357</v>
       </c>
     </row>
@@ -1754,7 +2009,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1765,61 +2020,76 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>School Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Average Math Score</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Average Reading Score</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>% Passing Math</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>% Passing Reading</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>% Overall Passing</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>83.47385187384614</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>83.89642074222549</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>93.62083003509466</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>96.58648927302872</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>90.43224369343228</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>76.95673306832398</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>80.96663632734915</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>66.54845257144746</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>80.79906211395057</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>53.67220822778149</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last update before submission, README + doc analysis
</commit_message>
<xml_diff>
--- a/personal-my-work/panda_challenge_analysis.xlsx
+++ b/personal-my-work/panda_challenge_analysis.xlsx
@@ -7,12 +7,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="per_school_summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="math_scores_by_grade" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="reading_scores_by_grad" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="spending_summary" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="size_summary" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="type_summary" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="district_summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="per_school_summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="math_scores_by_grade" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="reading_scores_by_grad" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="spending_summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="size_summary" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="type_summary" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -430,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,14 +440,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>school_name</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>School Type</t>
+          <t>Total Schools</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -456,638 +452,66 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Total School Budget</t>
+          <t>Total Budget</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Per Student Budget</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Average Math Score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Average Reading Score</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>% Passing Math</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>% Passing Reading</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
           <t>% Overall Passing</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Bailey High School</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4976</v>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>15</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>39,170</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$3,124,928.00</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>$628.00</t>
-        </is>
+          <t>$24,649,428.00</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>78.98537145774827</v>
       </c>
       <c r="F2" t="n">
-        <v>77.04843247588424</v>
+        <v>81.87784018381414</v>
       </c>
       <c r="G2" t="n">
-        <v>81.03396302250803</v>
+        <v>74.9808526933878</v>
       </c>
       <c r="H2" t="n">
-        <v>66.68006430868168</v>
+        <v>85.80546336482001</v>
       </c>
       <c r="I2" t="n">
-        <v>81.93327974276528</v>
-      </c>
-      <c r="J2" t="n">
-        <v>54.64228295819936</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Cabrera High School</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1858</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>$1,081,356.00</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>$582.00</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>83.06189451022605</v>
-      </c>
-      <c r="G3" t="n">
-        <v>83.97578040904197</v>
-      </c>
-      <c r="H3" t="n">
-        <v>94.1334768568353</v>
-      </c>
-      <c r="I3" t="n">
-        <v>97.03982777179763</v>
-      </c>
-      <c r="J3" t="n">
-        <v>91.33476856835307</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Figueroa High School</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2949</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>$1,884,411.00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>$639.00</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>76.71176670057646</v>
-      </c>
-      <c r="G4" t="n">
-        <v>81.15801966768396</v>
-      </c>
-      <c r="H4" t="n">
-        <v>65.98847066802306</v>
-      </c>
-      <c r="I4" t="n">
-        <v>80.73923363852153</v>
-      </c>
-      <c r="J4" t="n">
-        <v>53.20447609359105</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Ford High School</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2739</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>$1,763,916.00</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>$644.00</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>77.10259218692954</v>
-      </c>
-      <c r="G5" t="n">
-        <v>80.74625775830594</v>
-      </c>
-      <c r="H5" t="n">
-        <v>68.3096020445418</v>
-      </c>
-      <c r="I5" t="n">
-        <v>79.29901423877328</v>
-      </c>
-      <c r="J5" t="n">
-        <v>54.2898868200073</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Griffin High School</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1468</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>$917,500.00</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>$625.00</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>83.35149863760218</v>
-      </c>
-      <c r="G6" t="n">
-        <v>83.81675749318801</v>
-      </c>
-      <c r="H6" t="n">
-        <v>93.39237057220708</v>
-      </c>
-      <c r="I6" t="n">
-        <v>97.13896457765668</v>
-      </c>
-      <c r="J6" t="n">
-        <v>90.59945504087193</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Hernandez High School</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>4635</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>$3,022,020.00</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>$652.00</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>77.28975188781014</v>
-      </c>
-      <c r="G7" t="n">
-        <v>80.9344120819849</v>
-      </c>
-      <c r="H7" t="n">
-        <v>66.7529665587918</v>
-      </c>
-      <c r="I7" t="n">
-        <v>80.86299892125135</v>
-      </c>
-      <c r="J7" t="n">
-        <v>53.52750809061489</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Holden High School</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>427</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>$248,087.00</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>$581.00</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>83.80327868852459</v>
-      </c>
-      <c r="G8" t="n">
-        <v>83.81498829039812</v>
-      </c>
-      <c r="H8" t="n">
-        <v>92.50585480093677</v>
-      </c>
-      <c r="I8" t="n">
-        <v>96.25292740046838</v>
-      </c>
-      <c r="J8" t="n">
-        <v>89.22716627634661</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Huang High School</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>2917</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>$1,910,635.00</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>$655.00</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>76.62941378128214</v>
-      </c>
-      <c r="G9" t="n">
-        <v>81.18272197463148</v>
-      </c>
-      <c r="H9" t="n">
-        <v>65.68392183750429</v>
-      </c>
-      <c r="I9" t="n">
-        <v>81.31642098045937</v>
-      </c>
-      <c r="J9" t="n">
-        <v>53.51388412752829</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Johnson High School</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>4761</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>$3,094,650.00</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>$650.00</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>77.07246376811594</v>
-      </c>
-      <c r="G10" t="n">
-        <v>80.96639361478681</v>
-      </c>
-      <c r="H10" t="n">
-        <v>66.05755093467759</v>
-      </c>
-      <c r="I10" t="n">
-        <v>81.2224322621298</v>
-      </c>
-      <c r="J10" t="n">
-        <v>53.53917244276413</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Pena High School</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>962</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>$585,858.00</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>$609.00</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>83.83991683991684</v>
-      </c>
-      <c r="G11" t="n">
-        <v>84.04469854469855</v>
-      </c>
-      <c r="H11" t="n">
-        <v>94.5945945945946</v>
-      </c>
-      <c r="I11" t="n">
-        <v>95.94594594594595</v>
-      </c>
-      <c r="J11" t="n">
-        <v>90.54054054054055</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Rodriguez High School</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>District</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>3999</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>$2,547,363.00</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>$637.00</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>76.84271067766942</v>
-      </c>
-      <c r="G12" t="n">
-        <v>80.74468617154288</v>
-      </c>
-      <c r="H12" t="n">
-        <v>66.36659164791197</v>
-      </c>
-      <c r="I12" t="n">
-        <v>80.22005501375344</v>
-      </c>
-      <c r="J12" t="n">
-        <v>52.98824706176544</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Shelton High School</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1761</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>$1,056,600.00</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>$600.00</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>83.35945485519591</v>
-      </c>
-      <c r="G13" t="n">
-        <v>83.72572402044293</v>
-      </c>
-      <c r="H13" t="n">
-        <v>93.86712095400341</v>
-      </c>
-      <c r="I13" t="n">
-        <v>95.85462805224304</v>
-      </c>
-      <c r="J13" t="n">
-        <v>89.89210675752413</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Thomas High School</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1635</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>$1,043,130.00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>$638.00</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
-        <v>83.41834862385321</v>
-      </c>
-      <c r="G14" t="n">
-        <v>83.84892966360856</v>
-      </c>
-      <c r="H14" t="n">
-        <v>93.27217125382263</v>
-      </c>
-      <c r="I14" t="n">
-        <v>97.30886850152905</v>
-      </c>
-      <c r="J14" t="n">
-        <v>90.94801223241591</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Wilson High School</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>2283</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>$1,319,574.00</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>$578.00</t>
-        </is>
-      </c>
-      <c r="F15" t="n">
-        <v>83.2742006132282</v>
-      </c>
-      <c r="G15" t="n">
-        <v>83.98948751642575</v>
-      </c>
-      <c r="H15" t="n">
-        <v>93.86771791502409</v>
-      </c>
-      <c r="I15" t="n">
-        <v>96.53964082347788</v>
-      </c>
-      <c r="J15" t="n">
-        <v>90.5825667980727</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Wright High School</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Charter</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>$1,049,400.00</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>$583.00</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>83.68222222222222</v>
-      </c>
-      <c r="G16" t="n">
-        <v>83.955</v>
-      </c>
-      <c r="H16" t="n">
-        <v>93.33333333333333</v>
-      </c>
-      <c r="I16" t="n">
-        <v>96.61111111111111</v>
-      </c>
-      <c r="J16" t="n">
-        <v>90.33333333333333</v>
+        <v>65.17232575950983</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,24 +534,54 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>school_name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>9th</t>
+          <t>School Type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>10th</t>
+          <t>Total Students</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>11th</t>
+          <t>Total School Budget</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>12th</t>
+          <t>Per Student Budget</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Average Math Score</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Average Reading Score</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>% Passing Math</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>% Passing Reading</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>
@@ -1137,17 +591,38 @@
           <t>Bailey High School</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>77.08367626886145</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>76.99677158999192</v>
-      </c>
-      <c r="D2" t="n">
-        <v>77.51558752997602</v>
-      </c>
-      <c r="E2" t="n">
-        <v>76.49221789883268</v>
+        <v>4976</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$3,124,928.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>$628.00</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>77.04843247588424</v>
+      </c>
+      <c r="G2" t="n">
+        <v>81.03396302250803</v>
+      </c>
+      <c r="H2" t="n">
+        <v>66.68006430868168</v>
+      </c>
+      <c r="I2" t="n">
+        <v>81.93327974276528</v>
+      </c>
+      <c r="J2" t="n">
+        <v>54.64228295819936</v>
       </c>
     </row>
     <row r="3">
@@ -1156,17 +631,38 @@
           <t>Cabrera High School</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>83.09469696969697</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>83.15450643776823</v>
-      </c>
-      <c r="D3" t="n">
-        <v>82.7655601659751</v>
-      </c>
-      <c r="E3" t="n">
-        <v>83.27748691099477</v>
+        <v>1858</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$1,081,356.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$582.00</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>83.06189451022605</v>
+      </c>
+      <c r="G3" t="n">
+        <v>83.97578040904197</v>
+      </c>
+      <c r="H3" t="n">
+        <v>94.1334768568353</v>
+      </c>
+      <c r="I3" t="n">
+        <v>97.03982777179763</v>
+      </c>
+      <c r="J3" t="n">
+        <v>91.33476856835307</v>
       </c>
     </row>
     <row r="4">
@@ -1175,17 +671,38 @@
           <t>Figueroa High School</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>76.40303738317758</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C4" t="n">
-        <v>76.53997378768021</v>
-      </c>
-      <c r="D4" t="n">
-        <v>76.88434414668548</v>
-      </c>
-      <c r="E4" t="n">
-        <v>77.15136876006441</v>
+        <v>2949</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$1,884,411.00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$639.00</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>76.71176670057646</v>
+      </c>
+      <c r="G4" t="n">
+        <v>81.15801966768396</v>
+      </c>
+      <c r="H4" t="n">
+        <v>65.98847066802306</v>
+      </c>
+      <c r="I4" t="n">
+        <v>80.73923363852153</v>
+      </c>
+      <c r="J4" t="n">
+        <v>53.20447609359105</v>
       </c>
     </row>
     <row r="5">
@@ -1194,17 +711,38 @@
           <t>Ford High School</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>77.36134453781513</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>77.67231638418079</v>
-      </c>
-      <c r="D5" t="n">
-        <v>76.91805766312595</v>
-      </c>
-      <c r="E5" t="n">
-        <v>76.1799628942486</v>
+        <v>2739</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$1,763,916.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$644.00</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>77.10259218692954</v>
+      </c>
+      <c r="G5" t="n">
+        <v>80.74625775830594</v>
+      </c>
+      <c r="H5" t="n">
+        <v>68.3096020445418</v>
+      </c>
+      <c r="I5" t="n">
+        <v>79.29901423877328</v>
+      </c>
+      <c r="J5" t="n">
+        <v>54.2898868200073</v>
       </c>
     </row>
     <row r="6">
@@ -1213,17 +751,38 @@
           <t>Griffin High School</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>82.0440097799511</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C6" t="n">
-        <v>84.22906403940887</v>
-      </c>
-      <c r="D6" t="n">
-        <v>83.84210526315789</v>
-      </c>
-      <c r="E6" t="n">
-        <v>83.35616438356165</v>
+        <v>1468</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$917,500.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$625.00</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>83.35149863760218</v>
+      </c>
+      <c r="G6" t="n">
+        <v>83.81675749318801</v>
+      </c>
+      <c r="H6" t="n">
+        <v>93.39237057220708</v>
+      </c>
+      <c r="I6" t="n">
+        <v>97.13896457765668</v>
+      </c>
+      <c r="J6" t="n">
+        <v>90.59945504087193</v>
       </c>
     </row>
     <row r="7">
@@ -1232,17 +791,38 @@
           <t>Hernandez High School</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>77.43849493487699</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C7" t="n">
-        <v>77.33740831295843</v>
-      </c>
-      <c r="D7" t="n">
-        <v>77.13602941176471</v>
-      </c>
-      <c r="E7" t="n">
-        <v>77.18656716417911</v>
+        <v>4635</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$3,022,020.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$652.00</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>77.28975188781014</v>
+      </c>
+      <c r="G7" t="n">
+        <v>80.9344120819849</v>
+      </c>
+      <c r="H7" t="n">
+        <v>66.7529665587918</v>
+      </c>
+      <c r="I7" t="n">
+        <v>80.86299892125135</v>
+      </c>
+      <c r="J7" t="n">
+        <v>53.52750809061489</v>
       </c>
     </row>
     <row r="8">
@@ -1251,17 +831,38 @@
           <t>Holden High School</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>83.78740157480316</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C8" t="n">
-        <v>83.42982456140351</v>
-      </c>
-      <c r="D8" t="n">
-        <v>85</v>
-      </c>
-      <c r="E8" t="n">
-        <v>82.85542168674699</v>
+        <v>427</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$248,087.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$581.00</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>83.80327868852459</v>
+      </c>
+      <c r="G8" t="n">
+        <v>83.81498829039812</v>
+      </c>
+      <c r="H8" t="n">
+        <v>92.50585480093677</v>
+      </c>
+      <c r="I8" t="n">
+        <v>96.25292740046838</v>
+      </c>
+      <c r="J8" t="n">
+        <v>89.22716627634661</v>
       </c>
     </row>
     <row r="9">
@@ -1270,17 +871,38 @@
           <t>Huang High School</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>77.02725118483413</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C9" t="n">
-        <v>75.90873533246415</v>
-      </c>
-      <c r="D9" t="n">
-        <v>76.44660194174757</v>
-      </c>
-      <c r="E9" t="n">
-        <v>77.22564102564102</v>
+        <v>2917</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$1,910,635.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$655.00</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>76.62941378128214</v>
+      </c>
+      <c r="G9" t="n">
+        <v>81.18272197463148</v>
+      </c>
+      <c r="H9" t="n">
+        <v>65.68392183750429</v>
+      </c>
+      <c r="I9" t="n">
+        <v>81.31642098045937</v>
+      </c>
+      <c r="J9" t="n">
+        <v>53.51388412752829</v>
       </c>
     </row>
     <row r="10">
@@ -1289,17 +911,38 @@
           <t>Johnson High School</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>77.18785714285714</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C10" t="n">
-        <v>76.69111654441728</v>
-      </c>
-      <c r="D10" t="n">
-        <v>77.49165275459099</v>
-      </c>
-      <c r="E10" t="n">
-        <v>76.86324786324786</v>
+        <v>4761</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$3,094,650.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>$650.00</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>77.07246376811594</v>
+      </c>
+      <c r="G10" t="n">
+        <v>80.96639361478681</v>
+      </c>
+      <c r="H10" t="n">
+        <v>66.05755093467759</v>
+      </c>
+      <c r="I10" t="n">
+        <v>81.2224322621298</v>
+      </c>
+      <c r="J10" t="n">
+        <v>53.53917244276413</v>
       </c>
     </row>
     <row r="11">
@@ -1308,17 +951,38 @@
           <t>Pena High School</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>83.62545454545455</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C11" t="n">
-        <v>83.372</v>
-      </c>
-      <c r="D11" t="n">
-        <v>84.328125</v>
-      </c>
-      <c r="E11" t="n">
-        <v>84.12154696132596</v>
+        <v>962</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$585,858.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$609.00</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>83.83991683991684</v>
+      </c>
+      <c r="G11" t="n">
+        <v>84.04469854469855</v>
+      </c>
+      <c r="H11" t="n">
+        <v>94.5945945945946</v>
+      </c>
+      <c r="I11" t="n">
+        <v>95.94594594594595</v>
+      </c>
+      <c r="J11" t="n">
+        <v>90.54054054054055</v>
       </c>
     </row>
     <row r="12">
@@ -1327,17 +991,38 @@
           <t>Rodriguez High School</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>76.85996563573883</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
       </c>
       <c r="C12" t="n">
-        <v>76.6125</v>
-      </c>
-      <c r="D12" t="n">
-        <v>76.39562624254474</v>
-      </c>
-      <c r="E12" t="n">
-        <v>77.69074778200253</v>
+        <v>3999</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$2,547,363.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>$637.00</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>76.84271067766942</v>
+      </c>
+      <c r="G12" t="n">
+        <v>80.74468617154288</v>
+      </c>
+      <c r="H12" t="n">
+        <v>66.36659164791197</v>
+      </c>
+      <c r="I12" t="n">
+        <v>80.22005501375344</v>
+      </c>
+      <c r="J12" t="n">
+        <v>52.98824706176544</v>
       </c>
     </row>
     <row r="13">
@@ -1346,17 +1031,38 @@
           <t>Shelton High School</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>83.42075471698114</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C13" t="n">
-        <v>82.91741071428571</v>
-      </c>
-      <c r="D13" t="n">
-        <v>83.38349514563107</v>
-      </c>
-      <c r="E13" t="n">
-        <v>83.77897574123989</v>
+        <v>1761</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$1,056,600.00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>$600.00</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>83.35945485519591</v>
+      </c>
+      <c r="G13" t="n">
+        <v>83.72572402044293</v>
+      </c>
+      <c r="H13" t="n">
+        <v>93.86712095400341</v>
+      </c>
+      <c r="I13" t="n">
+        <v>95.85462805224304</v>
+      </c>
+      <c r="J13" t="n">
+        <v>89.89210675752413</v>
       </c>
     </row>
     <row r="14">
@@ -1365,17 +1071,38 @@
           <t>Thomas High School</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>83.59002169197397</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C14" t="n">
-        <v>83.08788598574822</v>
-      </c>
-      <c r="D14" t="n">
-        <v>83.49879518072289</v>
-      </c>
-      <c r="E14" t="n">
-        <v>83.49704142011835</v>
+        <v>1635</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$1,043,130.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$638.00</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>83.41834862385321</v>
+      </c>
+      <c r="G14" t="n">
+        <v>83.84892966360856</v>
+      </c>
+      <c r="H14" t="n">
+        <v>93.27217125382263</v>
+      </c>
+      <c r="I14" t="n">
+        <v>97.30886850152905</v>
+      </c>
+      <c r="J14" t="n">
+        <v>90.94801223241591</v>
       </c>
     </row>
     <row r="15">
@@ -1384,17 +1111,38 @@
           <t>Wilson High School</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>83.08557844690966</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C15" t="n">
-        <v>83.72442244224422</v>
-      </c>
-      <c r="D15" t="n">
-        <v>83.19532554257096</v>
-      </c>
-      <c r="E15" t="n">
-        <v>83.03579418344519</v>
+        <v>2283</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$1,319,574.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>$578.00</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>83.2742006132282</v>
+      </c>
+      <c r="G15" t="n">
+        <v>83.98948751642575</v>
+      </c>
+      <c r="H15" t="n">
+        <v>93.86771791502409</v>
+      </c>
+      <c r="I15" t="n">
+        <v>96.53964082347788</v>
+      </c>
+      <c r="J15" t="n">
+        <v>90.5825667980727</v>
       </c>
     </row>
     <row r="16">
@@ -1403,17 +1151,38 @@
           <t>Wright High School</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>83.26470588235294</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Charter</t>
+        </is>
       </c>
       <c r="C16" t="n">
-        <v>84.01028806584362</v>
-      </c>
-      <c r="D16" t="n">
-        <v>83.8367816091954</v>
-      </c>
-      <c r="E16" t="n">
-        <v>83.6449864498645</v>
+        <v>1800</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$1,049,400.00</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>$583.00</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>83.68222222222222</v>
+      </c>
+      <c r="G16" t="n">
+        <v>83.955</v>
+      </c>
+      <c r="H16" t="n">
+        <v>93.33333333333333</v>
+      </c>
+      <c r="I16" t="n">
+        <v>96.61111111111111</v>
+      </c>
+      <c r="J16" t="n">
+        <v>90.33333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -1464,16 +1233,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>81.30315500685872</v>
+        <v>77.08367626886145</v>
       </c>
       <c r="C2" t="n">
-        <v>80.90718321226795</v>
+        <v>76.99677158999192</v>
       </c>
       <c r="D2" t="n">
-        <v>80.94564348521183</v>
+        <v>77.51558752997602</v>
       </c>
       <c r="E2" t="n">
-        <v>80.91245136186771</v>
+        <v>76.49221789883268</v>
       </c>
     </row>
     <row r="3">
@@ -1483,16 +1252,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>83.67613636363636</v>
+        <v>83.09469696969697</v>
       </c>
       <c r="C3" t="n">
-        <v>84.25321888412017</v>
+        <v>83.15450643776823</v>
       </c>
       <c r="D3" t="n">
-        <v>83.78838174273859</v>
+        <v>82.7655601659751</v>
       </c>
       <c r="E3" t="n">
-        <v>84.28795811518324</v>
+        <v>83.27748691099477</v>
       </c>
     </row>
     <row r="4">
@@ -1502,16 +1271,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81.19859813084112</v>
+        <v>76.40303738317758</v>
       </c>
       <c r="C4" t="n">
-        <v>81.40891218872871</v>
+        <v>76.53997378768021</v>
       </c>
       <c r="D4" t="n">
-        <v>80.64033850493654</v>
+        <v>76.88434414668548</v>
       </c>
       <c r="E4" t="n">
-        <v>81.38486312399355</v>
+        <v>77.15136876006441</v>
       </c>
     </row>
     <row r="5">
@@ -1521,16 +1290,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>80.63265306122449</v>
+        <v>77.36134453781513</v>
       </c>
       <c r="C5" t="n">
-        <v>81.26271186440678</v>
+        <v>77.67231638418079</v>
       </c>
       <c r="D5" t="n">
-        <v>80.40364188163885</v>
+        <v>76.91805766312595</v>
       </c>
       <c r="E5" t="n">
-        <v>80.66233766233766</v>
+        <v>76.1799628942486</v>
       </c>
     </row>
     <row r="6">
@@ -1540,16 +1309,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>83.36919315403424</v>
+        <v>82.0440097799511</v>
       </c>
       <c r="C6" t="n">
-        <v>83.70689655172414</v>
+        <v>84.22906403940887</v>
       </c>
       <c r="D6" t="n">
-        <v>84.28808864265928</v>
+        <v>83.84210526315789</v>
       </c>
       <c r="E6" t="n">
-        <v>84.01369863013699</v>
+        <v>83.35616438356165</v>
       </c>
     </row>
     <row r="7">
@@ -1559,16 +1328,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>80.86685962373372</v>
+        <v>77.43849493487699</v>
       </c>
       <c r="C7" t="n">
-        <v>80.66014669926651</v>
+        <v>77.33740831295843</v>
       </c>
       <c r="D7" t="n">
-        <v>81.39613970588235</v>
+        <v>77.13602941176471</v>
       </c>
       <c r="E7" t="n">
-        <v>80.85714285714286</v>
+        <v>77.18656716417911</v>
       </c>
     </row>
     <row r="8">
@@ -1578,16 +1347,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>83.67716535433071</v>
+        <v>83.78740157480316</v>
       </c>
       <c r="C8" t="n">
-        <v>83.32456140350877</v>
+        <v>83.42982456140351</v>
       </c>
       <c r="D8" t="n">
-        <v>83.81553398058253</v>
+        <v>85</v>
       </c>
       <c r="E8" t="n">
-        <v>84.6987951807229</v>
+        <v>82.85542168674699</v>
       </c>
     </row>
     <row r="9">
@@ -1597,16 +1366,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>81.29028436018957</v>
+        <v>77.02725118483413</v>
       </c>
       <c r="C9" t="n">
-        <v>81.51238591916558</v>
+        <v>75.90873533246415</v>
       </c>
       <c r="D9" t="n">
-        <v>81.41747572815534</v>
+        <v>76.44660194174757</v>
       </c>
       <c r="E9" t="n">
-        <v>80.3059829059829</v>
+        <v>77.22564102564102</v>
       </c>
     </row>
     <row r="10">
@@ -1616,16 +1385,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>81.26071428571429</v>
+        <v>77.18785714285714</v>
       </c>
       <c r="C10" t="n">
-        <v>80.77343113284434</v>
+        <v>76.69111654441728</v>
       </c>
       <c r="D10" t="n">
-        <v>80.61602671118531</v>
+        <v>77.49165275459099</v>
       </c>
       <c r="E10" t="n">
-        <v>81.2275641025641</v>
+        <v>76.86324786324786</v>
       </c>
     </row>
     <row r="11">
@@ -1635,16 +1404,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>83.80727272727273</v>
+        <v>83.62545454545455</v>
       </c>
       <c r="C11" t="n">
-        <v>83.61199999999999</v>
+        <v>83.372</v>
       </c>
       <c r="D11" t="n">
-        <v>84.3359375</v>
+        <v>84.328125</v>
       </c>
       <c r="E11" t="n">
-        <v>84.59116022099448</v>
+        <v>84.12154696132596</v>
       </c>
     </row>
     <row r="12">
@@ -1654,16 +1423,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>80.99312714776632</v>
+        <v>76.85996563573883</v>
       </c>
       <c r="C12" t="n">
-        <v>80.62980769230769</v>
+        <v>76.6125</v>
       </c>
       <c r="D12" t="n">
-        <v>80.86481113320079</v>
+        <v>76.39562624254474</v>
       </c>
       <c r="E12" t="n">
-        <v>80.3764258555133</v>
+        <v>77.69074778200253</v>
       </c>
     </row>
     <row r="13">
@@ -1673,16 +1442,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>84.12264150943396</v>
+        <v>83.42075471698114</v>
       </c>
       <c r="C13" t="n">
-        <v>83.44196428571429</v>
+        <v>82.91741071428571</v>
       </c>
       <c r="D13" t="n">
-        <v>84.37378640776699</v>
+        <v>83.38349514563107</v>
       </c>
       <c r="E13" t="n">
-        <v>82.78167115902966</v>
+        <v>83.77897574123989</v>
       </c>
     </row>
     <row r="14">
@@ -1692,16 +1461,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>83.72885032537961</v>
+        <v>83.59002169197397</v>
       </c>
       <c r="C14" t="n">
-        <v>84.25415676959619</v>
+        <v>83.08788598574822</v>
       </c>
       <c r="D14" t="n">
-        <v>83.58554216867469</v>
+        <v>83.49879518072289</v>
       </c>
       <c r="E14" t="n">
-        <v>83.83136094674556</v>
+        <v>83.49704142011835</v>
       </c>
     </row>
     <row r="15">
@@ -1711,16 +1480,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>83.93977812995246</v>
+        <v>83.08557844690966</v>
       </c>
       <c r="C15" t="n">
-        <v>84.02145214521452</v>
+        <v>83.72442244224422</v>
       </c>
       <c r="D15" t="n">
-        <v>83.76460767946578</v>
+        <v>83.19532554257096</v>
       </c>
       <c r="E15" t="n">
-        <v>84.31767337807607</v>
+        <v>83.03579418344519</v>
       </c>
     </row>
     <row r="16">
@@ -1730,16 +1499,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>83.83333333333333</v>
+        <v>83.26470588235294</v>
       </c>
       <c r="C16" t="n">
-        <v>83.81275720164609</v>
+        <v>84.01028806584362</v>
       </c>
       <c r="D16" t="n">
-        <v>84.15632183908046</v>
+        <v>83.8367816091954</v>
       </c>
       <c r="E16" t="n">
-        <v>84.07317073170732</v>
+        <v>83.6449864498645</v>
       </c>
     </row>
   </sheetData>
@@ -1748,6 +1517,332 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>9th</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>10th</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>11th</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>12th</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Bailey High School</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>81.30315500685872</v>
+      </c>
+      <c r="C2" t="n">
+        <v>80.90718321226795</v>
+      </c>
+      <c r="D2" t="n">
+        <v>80.94564348521183</v>
+      </c>
+      <c r="E2" t="n">
+        <v>80.91245136186771</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Cabrera High School</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>83.67613636363636</v>
+      </c>
+      <c r="C3" t="n">
+        <v>84.25321888412017</v>
+      </c>
+      <c r="D3" t="n">
+        <v>83.78838174273859</v>
+      </c>
+      <c r="E3" t="n">
+        <v>84.28795811518324</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Figueroa High School</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>81.19859813084112</v>
+      </c>
+      <c r="C4" t="n">
+        <v>81.40891218872871</v>
+      </c>
+      <c r="D4" t="n">
+        <v>80.64033850493654</v>
+      </c>
+      <c r="E4" t="n">
+        <v>81.38486312399355</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Ford High School</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>80.63265306122449</v>
+      </c>
+      <c r="C5" t="n">
+        <v>81.26271186440678</v>
+      </c>
+      <c r="D5" t="n">
+        <v>80.40364188163885</v>
+      </c>
+      <c r="E5" t="n">
+        <v>80.66233766233766</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Griffin High School</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>83.36919315403424</v>
+      </c>
+      <c r="C6" t="n">
+        <v>83.70689655172414</v>
+      </c>
+      <c r="D6" t="n">
+        <v>84.28808864265928</v>
+      </c>
+      <c r="E6" t="n">
+        <v>84.01369863013699</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Hernandez High School</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>80.86685962373372</v>
+      </c>
+      <c r="C7" t="n">
+        <v>80.66014669926651</v>
+      </c>
+      <c r="D7" t="n">
+        <v>81.39613970588235</v>
+      </c>
+      <c r="E7" t="n">
+        <v>80.85714285714286</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Holden High School</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>83.67716535433071</v>
+      </c>
+      <c r="C8" t="n">
+        <v>83.32456140350877</v>
+      </c>
+      <c r="D8" t="n">
+        <v>83.81553398058253</v>
+      </c>
+      <c r="E8" t="n">
+        <v>84.6987951807229</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Huang High School</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>81.29028436018957</v>
+      </c>
+      <c r="C9" t="n">
+        <v>81.51238591916558</v>
+      </c>
+      <c r="D9" t="n">
+        <v>81.41747572815534</v>
+      </c>
+      <c r="E9" t="n">
+        <v>80.3059829059829</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Johnson High School</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>81.26071428571429</v>
+      </c>
+      <c r="C10" t="n">
+        <v>80.77343113284434</v>
+      </c>
+      <c r="D10" t="n">
+        <v>80.61602671118531</v>
+      </c>
+      <c r="E10" t="n">
+        <v>81.2275641025641</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Pena High School</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>83.80727272727273</v>
+      </c>
+      <c r="C11" t="n">
+        <v>83.61199999999999</v>
+      </c>
+      <c r="D11" t="n">
+        <v>84.3359375</v>
+      </c>
+      <c r="E11" t="n">
+        <v>84.59116022099448</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Rodriguez High School</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>80.99312714776632</v>
+      </c>
+      <c r="C12" t="n">
+        <v>80.62980769230769</v>
+      </c>
+      <c r="D12" t="n">
+        <v>80.86481113320079</v>
+      </c>
+      <c r="E12" t="n">
+        <v>80.3764258555133</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Shelton High School</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>84.12264150943396</v>
+      </c>
+      <c r="C13" t="n">
+        <v>83.44196428571429</v>
+      </c>
+      <c r="D13" t="n">
+        <v>84.37378640776699</v>
+      </c>
+      <c r="E13" t="n">
+        <v>82.78167115902966</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Thomas High School</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>83.72885032537961</v>
+      </c>
+      <c r="C14" t="n">
+        <v>84.25415676959619</v>
+      </c>
+      <c r="D14" t="n">
+        <v>83.58554216867469</v>
+      </c>
+      <c r="E14" t="n">
+        <v>83.83136094674556</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Wilson High School</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>83.93977812995246</v>
+      </c>
+      <c r="C15" t="n">
+        <v>84.02145214521452</v>
+      </c>
+      <c r="D15" t="n">
+        <v>83.76460767946578</v>
+      </c>
+      <c r="E15" t="n">
+        <v>84.31767337807607</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Wright High School</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>83.83333333333333</v>
+      </c>
+      <c r="C16" t="n">
+        <v>83.81275720164609</v>
+      </c>
+      <c r="D16" t="n">
+        <v>84.15632183908046</v>
+      </c>
+      <c r="E16" t="n">
+        <v>84.07317073170732</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1886,7 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2003,7 +2098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>